<commit_message>
Added testdata and excel file
</commit_message>
<xml_diff>
--- a/testng-appium-app-browserstack-sdk/android/testng-examples/src/test/java/com/myBank/testdata/testdata.xlsx
+++ b/testng-appium-app-browserstack-sdk/android/testng-examples/src/test/java/com/myBank/testdata/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="17544" windowHeight="8280"/>
+    <workbookView windowWidth="19128" windowHeight="9407" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="66">
   <si>
     <t>Name</t>
   </si>
@@ -44,6 +44,9 @@
     <t>cyrilshaji38@gmail.com</t>
   </si>
   <si>
+    <t>1234567890</t>
+  </si>
+  <si>
     <t>ABC09876543</t>
   </si>
   <si>
@@ -68,6 +71,9 @@
     <t>karen99@gmail.com</t>
   </si>
   <si>
+    <t>1234567895</t>
+  </si>
+  <si>
     <t>CAB54321098</t>
   </si>
   <si>
@@ -80,6 +86,9 @@
     <t>chandichen@gmail.com</t>
   </si>
   <si>
+    <t>1234567893</t>
+  </si>
+  <si>
     <t>ABC76543210</t>
   </si>
   <si>
@@ -92,6 +101,9 @@
     <t>nakki2000@gmail.com</t>
   </si>
   <si>
+    <t>1234567894</t>
+  </si>
+  <si>
     <t>BCA65432109</t>
   </si>
   <si>
@@ -104,6 +116,9 @@
     <t>chandnisuresh2000@gmail.com</t>
   </si>
   <si>
+    <t>1234567891</t>
+  </si>
+  <si>
     <t>BCA98765432</t>
   </si>
   <si>
@@ -116,6 +131,9 @@
     <t>alku99@gmail.com</t>
   </si>
   <si>
+    <t>1234567897</t>
+  </si>
+  <si>
     <t>BCA32109876</t>
   </si>
   <si>
@@ -128,6 +146,9 @@
     <t>raju99@gmail.com</t>
   </si>
   <si>
+    <t>1234567899</t>
+  </si>
+  <si>
     <t>ABC10987654</t>
   </si>
   <si>
@@ -140,6 +161,9 @@
     <t>ashwinpp@gmail.com</t>
   </si>
   <si>
+    <t>1234567898</t>
+  </si>
+  <si>
     <t>CAB21098765</t>
   </si>
   <si>
@@ -152,10 +176,43 @@
     <t>meenu99@gmail.com</t>
   </si>
   <si>
+    <t>1234567892</t>
+  </si>
+  <si>
     <t>CAB87654321</t>
   </si>
   <si>
     <t>amount</t>
+  </si>
+  <si>
+    <t>100.000</t>
+  </si>
+  <si>
+    <t>200.00</t>
+  </si>
+  <si>
+    <t>300.00</t>
+  </si>
+  <si>
+    <t>400.00</t>
+  </si>
+  <si>
+    <t>500.00</t>
+  </si>
+  <si>
+    <t>600.00</t>
+  </si>
+  <si>
+    <t>700.00</t>
+  </si>
+  <si>
+    <t>800.00</t>
+  </si>
+  <si>
+    <t>900.00</t>
+  </si>
+  <si>
+    <t>1000.00</t>
   </si>
 </sst>
 </file>
@@ -163,11 +220,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="0.00_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="0.00_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -180,6 +237,29 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -187,7 +267,67 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -201,16 +341,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -218,98 +366,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -331,49 +388,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -385,133 +526,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -527,9 +584,20 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -545,6 +613,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -602,40 +679,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -645,130 +702,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -776,16 +833,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1109,14 +1169,14 @@
   <sheetPr/>
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="11.2222222222222" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="2" max="2" width="28.7777777777778" customWidth="1"/>
     <col min="3" max="3" width="29.6666666666667" customWidth="1"/>
     <col min="4" max="4" width="14.8888888888889" customWidth="1"/>
     <col min="5" max="5" width="16.5555555555556" customWidth="1"/>
@@ -1153,11 +1213,11 @@
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2">
-        <v>1234567890</v>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="3">
         <v>15200</v>
@@ -1165,19 +1225,19 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3">
-        <v>1234567896</v>
+        <v>13</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3" s="3">
         <v>5936</v>
@@ -1185,19 +1245,19 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4">
-        <v>1234567895</v>
+        <v>17</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F4" s="3">
         <v>1194.16</v>
@@ -1205,19 +1265,19 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5">
-        <v>1234567893</v>
+        <v>22</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F5" s="3">
         <v>1650.01</v>
@@ -1225,19 +1285,19 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6">
-        <v>1234567894</v>
+        <v>27</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F6" s="3">
         <v>2004.48</v>
@@ -1245,19 +1305,19 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7">
-        <v>1234567891</v>
+        <v>32</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F7" s="3">
         <v>10582.7</v>
@@ -1265,19 +1325,19 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8">
-        <v>1234567897</v>
+        <v>37</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="F8">
         <v>857.22</v>
@@ -1285,19 +1345,19 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9">
-        <v>1234567899</v>
+        <v>42</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="F9">
         <v>273.9</v>
@@ -1305,19 +1365,19 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10">
-        <v>1234567898</v>
+        <v>47</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="E10" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="F10" s="3">
         <v>4398.46</v>
@@ -1325,19 +1385,19 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11">
-        <v>1234567892</v>
+        <v>52</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="E11" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="F11" s="3">
         <v>1359.56</v>
@@ -1358,65 +1418,65 @@
   <sheetPr/>
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="1">
-        <v>100</v>
+      <c r="A2" s="5" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="1">
-        <v>200</v>
+      <c r="A3" s="5" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="1">
-        <v>300</v>
+      <c r="A4" s="5" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="1">
-        <v>400</v>
+      <c r="A5" s="5" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="1">
-        <v>500</v>
+      <c r="A6" s="5" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="1">
-        <v>600</v>
+      <c r="A7" s="5" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="1">
-        <v>700</v>
+      <c r="A8" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="1">
-        <v>800</v>
+      <c r="A9" s="5" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="1">
-        <v>900</v>
+      <c r="A10" s="5" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="1">
-        <v>1000</v>
+      <c r="A11" s="5" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update page object model
</commit_message>
<xml_diff>
--- a/testng-appium-app-browserstack-sdk/android/testng-examples/src/test/java/com/myBank/testdata/testdata.xlsx
+++ b/testng-appium-app-browserstack-sdk/android/testng-examples/src/test/java/com/myBank/testdata/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19128" windowHeight="9407" activeTab="1"/>
+    <workbookView windowWidth="18695" windowHeight="8280" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -182,37 +182,13 @@
     <t>CAB87654321</t>
   </si>
   <si>
+    <t>Herald</t>
+  </si>
+  <si>
+    <t>ABCD1234</t>
+  </si>
+  <si>
     <t>amount</t>
-  </si>
-  <si>
-    <t>100.000</t>
-  </si>
-  <si>
-    <t>200.00</t>
-  </si>
-  <si>
-    <t>300.00</t>
-  </si>
-  <si>
-    <t>400.00</t>
-  </si>
-  <si>
-    <t>500.00</t>
-  </si>
-  <si>
-    <t>600.00</t>
-  </si>
-  <si>
-    <t>700.00</t>
-  </si>
-  <si>
-    <t>800.00</t>
-  </si>
-  <si>
-    <t>900.00</t>
-  </si>
-  <si>
-    <t>1000.00</t>
   </si>
 </sst>
 </file>
@@ -220,11 +196,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="0.00_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="0.00_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -250,38 +226,61 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -296,44 +295,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -350,7 +311,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -358,6 +319,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -366,7 +335,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -388,25 +364,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -418,126 +514,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -551,18 +539,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -584,20 +560,24 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -651,21 +631,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -679,20 +644,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -702,130 +678,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -843,9 +819,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1167,10 +1140,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -1220,7 +1193,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="3">
-        <v>15200</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1260,7 +1233,7 @@
         <v>19</v>
       </c>
       <c r="F4" s="3">
-        <v>1194.16</v>
+        <v>945.16</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1280,7 +1253,7 @@
         <v>24</v>
       </c>
       <c r="F5" s="3">
-        <v>1650.01</v>
+        <v>1500.01</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1300,7 +1273,7 @@
         <v>29</v>
       </c>
       <c r="F6" s="3">
-        <v>2004.48</v>
+        <v>2603.48</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1401,6 +1374,17 @@
       </c>
       <c r="F11" s="3">
         <v>1359.56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -1416,67 +1400,87 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="5" t="s">
-        <v>56</v>
+      <c r="A2" s="1">
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="5" t="s">
-        <v>57</v>
+      <c r="A3" s="1">
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="5" t="s">
-        <v>58</v>
+      <c r="A4" s="1">
+        <v>300</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="5" t="s">
-        <v>59</v>
+      <c r="A5" s="1">
+        <v>400</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="5" t="s">
-        <v>60</v>
+      <c r="A6" s="1">
+        <v>500</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="5" t="s">
-        <v>61</v>
+      <c r="A7" s="1">
+        <v>600</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="5" t="s">
-        <v>62</v>
+      <c r="A8" s="1">
+        <v>700</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="5" t="s">
-        <v>63</v>
+      <c r="A9" s="1">
+        <v>800</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="5" t="s">
-        <v>64</v>
+      <c r="A10" s="1">
+        <v>900</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="5" t="s">
-        <v>65</v>
+      <c r="A11" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="1">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="1">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="1">
+        <v>5000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>